<commit_message>
nowe wersje i poprawki
</commit_message>
<xml_diff>
--- a/Statystyki_2018/Template/okrp.xlsx
+++ b/Statystyki_2018/Template/okrp.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myProjects\prv\statystyki\Statystyki_2018\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBABA81-431C-4328-B92B-E39C88632C0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC335BE-68E3-415A-878B-CAA855A56394}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="174" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="174" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Lp.</t>
   </si>
@@ -90,15 +90,6 @@
   </si>
   <si>
     <t>WSC</t>
-  </si>
-  <si>
-    <t>miesiąc</t>
-  </si>
-  <si>
-    <t>sąd</t>
-  </si>
-  <si>
-    <t>wydział</t>
   </si>
   <si>
     <t>Razem</t>
@@ -158,6 +149,12 @@
   </si>
   <si>
     <t>Terminowość sporządzonych uzasadnień orzeczeń merytorycznych C i Ns</t>
+  </si>
+  <si>
+    <t>Pz</t>
+  </si>
+  <si>
+    <t>Uz</t>
   </si>
 </sst>
 </file>
@@ -263,7 +260,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,12 +275,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="22"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="31"/>
         <bgColor indexed="22"/>
       </patternFill>
@@ -513,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -530,43 +521,16 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -581,6 +545,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -588,6 +573,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -596,7 +584,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1066,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1078,28 +1066,29 @@
     <col min="3" max="3" width="32.77734375" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
     <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="30" max="32" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:31" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="15" t="s">
@@ -1116,7 +1105,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
@@ -1137,158 +1126,152 @@
       <c r="AB1" s="18"/>
       <c r="AC1" s="18"/>
       <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="19" t="s">
+      <c r="AE1" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="20" t="s">
+    <row r="2" spans="1:31" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="17"/>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="17"/>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="7" t="s">
+      <c r="U2" s="20"/>
+      <c r="V2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="7" t="s">
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="14" t="s">
         <v>21</v>
       </c>
       <c r="AA2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AD2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AE2" s="10"/>
+    </row>
+    <row r="3" spans="1:31" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF2" s="19"/>
-    </row>
-    <row r="3" spans="1:32" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="N3" s="17"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="11"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="19"/>
       <c r="R3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S3" s="17"/>
       <c r="T3" s="4"/>
       <c r="U3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
+      <c r="AC3" s="14"/>
       <c r="AD3" s="9"/>
       <c r="AE3" s="10"/>
-      <c r="AF3" s="19"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="32">
+  <mergeCells count="31">
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="G1:G3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:N3"/>
-    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="T1:AD1"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1303,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1314,84 +1297,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26" t="s">
-        <v>35</v>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="28" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="26" t="s">
+      <c r="I3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="26"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+        <v>40</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>